<commit_message>
Update: minor requirement fix
</commit_message>
<xml_diff>
--- a/dad5_smertebehandling_v100_export.xlsx
+++ b/dad5_smertebehandling_v100_export.xlsx
@@ -540,6 +540,11 @@
           <t>Typen og Dato I forhold til smertebehandling som patienten har modtaget</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="D5" t="inlineStr">

</xml_diff>